<commit_message>
Entities for project first commit
</commit_message>
<xml_diff>
--- a/Grp-18_e-Tour.xlsx
+++ b/Grp-18_e-Tour.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="194">
   <si>
     <t>daysID</t>
   </si>
@@ -447,9 +447,6 @@
     <t>itr-dtl</t>
   </si>
   <si>
-    <t>Pk, auto</t>
-  </si>
-  <si>
     <t>details</t>
   </si>
   <si>
@@ -504,12 +501,6 @@
     <t>cust-id</t>
   </si>
   <si>
-    <t>cust-name</t>
-  </si>
-  <si>
-    <t>cust-details</t>
-  </si>
-  <si>
     <t>Package Master</t>
   </si>
   <si>
@@ -556,6 +547,57 @@
   </si>
   <si>
     <t>Tour Categoty Master</t>
+  </si>
+  <si>
+    <t>cust-FirstName</t>
+  </si>
+  <si>
+    <t>cust-Middle Name</t>
+  </si>
+  <si>
+    <t>cust-LastName</t>
+  </si>
+  <si>
+    <t>cust-age</t>
+  </si>
+  <si>
+    <t>cust-phonenumber</t>
+  </si>
+  <si>
+    <t>cust-email</t>
+  </si>
+  <si>
+    <t>cust-idproof</t>
+  </si>
+  <si>
+    <t>cust-idproofnumber</t>
+  </si>
+  <si>
+    <t>cust-RoomNo</t>
+  </si>
+  <si>
+    <t>cust-BuildingName</t>
+  </si>
+  <si>
+    <t>cust-Street</t>
+  </si>
+  <si>
+    <t>cust-Area</t>
+  </si>
+  <si>
+    <t>cust-City</t>
+  </si>
+  <si>
+    <t>cust-state</t>
+  </si>
+  <si>
+    <t>cust-pin</t>
+  </si>
+  <si>
+    <t>costwithsharing person</t>
+  </si>
+  <si>
+    <t>repeat</t>
   </si>
 </sst>
 </file>
@@ -602,7 +644,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,6 +672,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,7 +784,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -828,7 +876,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -840,28 +895,39 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1166,7 +1232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U154"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
@@ -1194,26 +1260,26 @@
       <c r="A1" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="44"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1286,15 +1352,15 @@
       <c r="H7" s="1"/>
     </row>
     <row r="10" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:17" ht="18" x14ac:dyDescent="0.3">
@@ -1349,13 +1415,13 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="13"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="42"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="48"/>
     </row>
     <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
@@ -1507,15 +1573,15 @@
       <c r="Q19" s="26"/>
     </row>
     <row r="20" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
       <c r="K20" s="26"/>
       <c r="L20" s="26"/>
       <c r="M20" s="25"/>
@@ -1641,15 +1707,15 @@
     </row>
     <row r="26" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="B26" s="1"/>
-      <c r="C26" s="43" t="s">
+      <c r="C26" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="13"/>
@@ -1741,15 +1807,15 @@
       <c r="N31" s="13"/>
     </row>
     <row r="32" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="43"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
       <c r="J32" s="1"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
@@ -1879,15 +1945,15 @@
       <c r="O40" s="1"/>
     </row>
     <row r="41" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="39"/>
-      <c r="F41" s="39"/>
-      <c r="G41" s="40"/>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="43"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="13"/>
@@ -1969,8 +2035,8 @@
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
-      <c r="L44" s="37"/>
-      <c r="M44" s="37"/>
+      <c r="L44" s="46"/>
+      <c r="M44" s="46"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
     </row>
@@ -2066,15 +2132,15 @@
     </row>
     <row r="51" spans="2:21" ht="18" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B51" s="1"/>
-      <c r="C51" s="43" t="s">
+      <c r="C51" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="44"/>
     </row>
     <row r="52" spans="2:21" ht="18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
@@ -2162,15 +2228,15 @@
       <c r="I56" s="12"/>
     </row>
     <row r="57" spans="2:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="C57" s="43" t="s">
+      <c r="C57" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="D57" s="43"/>
-      <c r="E57" s="43"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="43"/>
-      <c r="H57" s="43"/>
-      <c r="I57" s="43"/>
+      <c r="D57" s="44"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="44"/>
+      <c r="G57" s="44"/>
+      <c r="H57" s="44"/>
+      <c r="I57" s="44"/>
     </row>
     <row r="58" spans="2:21" ht="18" x14ac:dyDescent="0.3">
       <c r="C58" s="8" t="s">
@@ -2234,12 +2300,12 @@
       <c r="M60" s="13"/>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
-      <c r="P60" s="37"/>
-      <c r="Q60" s="37"/>
-      <c r="R60" s="37"/>
-      <c r="S60" s="37"/>
-      <c r="T60" s="37"/>
-      <c r="U60" s="37"/>
+      <c r="P60" s="46"/>
+      <c r="Q60" s="46"/>
+      <c r="R60" s="46"/>
+      <c r="S60" s="46"/>
+      <c r="T60" s="46"/>
+      <c r="U60" s="46"/>
     </row>
     <row r="61" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C61" s="17"/>
@@ -2284,15 +2350,15 @@
       <c r="U62" s="13"/>
     </row>
     <row r="63" spans="2:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="C63" s="43" t="s">
+      <c r="C63" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="D63" s="43"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="43"/>
-      <c r="G63" s="43"/>
-      <c r="H63" s="43"/>
-      <c r="I63" s="43"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="44"/>
+      <c r="H63" s="44"/>
+      <c r="I63" s="44"/>
       <c r="J63" s="1"/>
       <c r="K63" s="17"/>
       <c r="L63" s="17"/>
@@ -2451,15 +2517,15 @@
       <c r="O69" s="13"/>
     </row>
     <row r="71" spans="1:21" ht="18" x14ac:dyDescent="0.35">
-      <c r="A71" s="38" t="s">
+      <c r="A71" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B71" s="39"/>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="39"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="40"/>
+      <c r="B71" s="42"/>
+      <c r="C71" s="42"/>
+      <c r="D71" s="42"/>
+      <c r="E71" s="42"/>
+      <c r="F71" s="42"/>
+      <c r="G71" s="43"/>
     </row>
     <row r="72" spans="1:21" ht="18" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
@@ -2486,8 +2552,8 @@
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
       <c r="J72" s="1"/>
-      <c r="K72" s="37"/>
-      <c r="L72" s="37"/>
+      <c r="K72" s="46"/>
+      <c r="L72" s="46"/>
       <c r="M72" s="1"/>
     </row>
     <row r="73" spans="1:21" ht="18" x14ac:dyDescent="0.35">
@@ -2766,15 +2832,15 @@
       <c r="G88" s="12"/>
     </row>
     <row r="89" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="C89" s="38" t="s">
+      <c r="C89" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="D89" s="39"/>
-      <c r="E89" s="39"/>
-      <c r="F89" s="39"/>
-      <c r="G89" s="39"/>
-      <c r="H89" s="39"/>
-      <c r="I89" s="40"/>
+      <c r="D89" s="42"/>
+      <c r="E89" s="42"/>
+      <c r="F89" s="42"/>
+      <c r="G89" s="42"/>
+      <c r="H89" s="42"/>
+      <c r="I89" s="43"/>
     </row>
     <row r="90" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="C90" s="8" t="s">
@@ -2869,15 +2935,15 @@
     <row r="96" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A96" s="22"/>
       <c r="B96" s="12"/>
-      <c r="C96" s="38" t="s">
+      <c r="C96" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="D96" s="39"/>
-      <c r="E96" s="39"/>
-      <c r="F96" s="39"/>
-      <c r="G96" s="39"/>
-      <c r="H96" s="39"/>
-      <c r="I96" s="40"/>
+      <c r="D96" s="42"/>
+      <c r="E96" s="42"/>
+      <c r="F96" s="42"/>
+      <c r="G96" s="42"/>
+      <c r="H96" s="42"/>
+      <c r="I96" s="43"/>
     </row>
     <row r="97" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A97" s="12"/>
@@ -3031,15 +3097,15 @@
     <row r="106" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A106" s="22"/>
       <c r="B106" s="12"/>
-      <c r="C106" s="38" t="s">
+      <c r="C106" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="D106" s="39"/>
-      <c r="E106" s="39"/>
-      <c r="F106" s="39"/>
-      <c r="G106" s="39"/>
-      <c r="H106" s="39"/>
-      <c r="I106" s="40"/>
+      <c r="D106" s="42"/>
+      <c r="E106" s="42"/>
+      <c r="F106" s="42"/>
+      <c r="G106" s="42"/>
+      <c r="H106" s="42"/>
+      <c r="I106" s="43"/>
     </row>
     <row r="107" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A107" s="22"/>
@@ -3119,15 +3185,15 @@
       <c r="G111" s="13"/>
     </row>
     <row r="112" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="C112" s="38" t="s">
+      <c r="C112" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="D112" s="39"/>
-      <c r="E112" s="39"/>
-      <c r="F112" s="39"/>
-      <c r="G112" s="39"/>
-      <c r="H112" s="39"/>
-      <c r="I112" s="40"/>
+      <c r="D112" s="42"/>
+      <c r="E112" s="42"/>
+      <c r="F112" s="42"/>
+      <c r="G112" s="42"/>
+      <c r="H112" s="42"/>
+      <c r="I112" s="43"/>
     </row>
     <row r="113" spans="1:17" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="C113" s="8" t="s">
@@ -3196,15 +3262,15 @@
       <c r="I116" s="12"/>
     </row>
     <row r="119" spans="1:17" ht="18" x14ac:dyDescent="0.35">
-      <c r="A119" s="38" t="s">
+      <c r="A119" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="39"/>
-      <c r="F119" s="39"/>
-      <c r="G119" s="40"/>
+      <c r="B119" s="42"/>
+      <c r="C119" s="42"/>
+      <c r="D119" s="42"/>
+      <c r="E119" s="42"/>
+      <c r="F119" s="42"/>
+      <c r="G119" s="43"/>
     </row>
     <row r="120" spans="1:17" ht="18" x14ac:dyDescent="0.3">
       <c r="A120" s="8" t="s">
@@ -3395,15 +3461,15 @@
       <c r="G132" s="17"/>
     </row>
     <row r="133" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="C133" s="38" t="s">
+      <c r="C133" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="D133" s="39"/>
-      <c r="E133" s="39"/>
-      <c r="F133" s="39"/>
-      <c r="G133" s="39"/>
-      <c r="H133" s="39"/>
-      <c r="I133" s="40"/>
+      <c r="D133" s="42"/>
+      <c r="E133" s="42"/>
+      <c r="F133" s="42"/>
+      <c r="G133" s="42"/>
+      <c r="H133" s="42"/>
+      <c r="I133" s="43"/>
     </row>
     <row r="134" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="C134" s="8" t="s">
@@ -3536,15 +3602,15 @@
       <c r="I141" s="12"/>
     </row>
     <row r="143" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="C143" s="38" t="s">
+      <c r="C143" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="D143" s="39"/>
-      <c r="E143" s="39"/>
-      <c r="F143" s="39"/>
-      <c r="G143" s="39"/>
-      <c r="H143" s="39"/>
-      <c r="I143" s="40"/>
+      <c r="D143" s="42"/>
+      <c r="E143" s="42"/>
+      <c r="F143" s="42"/>
+      <c r="G143" s="42"/>
+      <c r="H143" s="42"/>
+      <c r="I143" s="43"/>
     </row>
     <row r="144" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="C144" s="8" t="s">
@@ -3650,15 +3716,15 @@
       <c r="G150" s="12"/>
     </row>
     <row r="151" spans="3:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="C151" s="38" t="s">
+      <c r="C151" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="D151" s="39"/>
-      <c r="E151" s="39"/>
-      <c r="F151" s="39"/>
-      <c r="G151" s="39"/>
-      <c r="H151" s="39"/>
-      <c r="I151" s="40"/>
+      <c r="D151" s="42"/>
+      <c r="E151" s="42"/>
+      <c r="F151" s="42"/>
+      <c r="G151" s="42"/>
+      <c r="H151" s="42"/>
+      <c r="I151" s="43"/>
     </row>
     <row r="152" spans="3:9" ht="18" x14ac:dyDescent="0.3">
       <c r="C152" s="8" t="s">
@@ -3719,19 +3785,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C133:I133"/>
-    <mergeCell ref="C143:I143"/>
-    <mergeCell ref="C151:I151"/>
-    <mergeCell ref="C89:I89"/>
-    <mergeCell ref="C96:I96"/>
-    <mergeCell ref="C106:I106"/>
-    <mergeCell ref="C112:I112"/>
-    <mergeCell ref="A119:G119"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
     <mergeCell ref="P60:U60"/>
     <mergeCell ref="K72:L72"/>
     <mergeCell ref="A71:G71"/>
@@ -3743,6 +3796,19 @@
     <mergeCell ref="C32:I32"/>
     <mergeCell ref="A41:G41"/>
     <mergeCell ref="C63:I63"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="C133:I133"/>
+    <mergeCell ref="C143:I143"/>
+    <mergeCell ref="C151:I151"/>
+    <mergeCell ref="C89:I89"/>
+    <mergeCell ref="C96:I96"/>
+    <mergeCell ref="C106:I106"/>
+    <mergeCell ref="C112:I112"/>
+    <mergeCell ref="A119:G119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3751,15 +3817,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G105"/>
+  <dimension ref="A2:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
@@ -3768,114 +3834,114 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="A2" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="37" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="52">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="52">
         <v>3</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="52">
         <v>3</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
@@ -4114,88 +4180,88 @@
       <c r="G28" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="45" t="s">
+      <c r="D31" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="E31" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F31" s="45" t="s">
+      <c r="F31" s="37" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46" t="s">
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52" t="s">
+        <v>193</v>
+      </c>
+      <c r="F33" s="52"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="52">
+        <v>2</v>
+      </c>
+      <c r="D34" s="52"/>
+      <c r="E34" s="52"/>
+      <c r="F34" s="52"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="3">
-        <v>2</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F35" s="3"/>
+      <c r="F35" s="52"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
@@ -4214,226 +4280,220 @@
       <c r="F37" s="36"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="48" t="s">
+      <c r="A39" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" s="49"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" s="37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="45" t="s">
+      <c r="B41" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="52"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="52">
+        <v>5</v>
+      </c>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="52">
+        <v>3</v>
+      </c>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="53" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="52">
+        <v>3</v>
+      </c>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="B45" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+    </row>
+    <row r="46" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="53" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="52"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+    </row>
+    <row r="47" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="53" t="s">
+        <v>157</v>
+      </c>
+      <c r="B47" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="52"/>
+      <c r="D47" s="52"/>
+      <c r="E47" s="52"/>
+      <c r="F47" s="52"/>
+    </row>
+    <row r="48" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="B48" s="52"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+    </row>
+    <row r="49" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="52"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="52"/>
+      <c r="F49" s="52"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="53" t="s">
+        <v>149</v>
+      </c>
+      <c r="B50" s="52" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="49" t="s">
+        <v>150</v>
+      </c>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="49"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="B40" s="45" t="s">
+      <c r="B55" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="C40" s="45" t="s">
+      <c r="C55" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="D40" s="45" t="s">
+      <c r="D55" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E40" s="45" t="s">
+      <c r="E55" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F40" s="45" t="s">
+      <c r="F55" s="37" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="B41" s="46" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="3">
-        <v>5</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="3">
-        <v>3</v>
-      </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44" s="3">
-        <v>3</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-    </row>
-    <row r="48" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="47" t="s">
-        <v>150</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="48" t="s">
-        <v>151</v>
-      </c>
-      <c r="B53" s="48"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="48"/>
-      <c r="E53" s="48"/>
-      <c r="F53" s="48"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="B54" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="C54" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="D54" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E54" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F54" s="45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="B55" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C55" s="46"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="46"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C56" s="3">
-        <v>5</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C57" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
+      <c r="E57" s="3" t="s">
+        <v>193</v>
+      </c>
       <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>39</v>
@@ -4447,374 +4507,579 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C59" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="C59" s="3">
+        <v>3</v>
+      </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="48" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="49" t="s">
+        <v>159</v>
+      </c>
+      <c r="B66" s="49"/>
+      <c r="C66" s="49"/>
+      <c r="D66" s="49"/>
+      <c r="E66" s="49"/>
+      <c r="F66" s="49"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B67" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C67" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E67" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="F67" s="37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="B65" s="48"/>
-      <c r="C65" s="48"/>
-      <c r="D65" s="48"/>
-      <c r="E65" s="48"/>
-      <c r="F65" s="48"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="B66" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="C66" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="D66" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E66" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F66" s="45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="46" t="s">
-        <v>161</v>
-      </c>
-      <c r="B67" s="46" t="s">
+      <c r="B68" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C67" s="46"/>
-      <c r="D67" s="46" t="s">
+      <c r="C68" s="38"/>
+      <c r="D68" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="E67" s="46"/>
-      <c r="F67" s="46"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B69" s="3"/>
+        <v>177</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="48" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B71" s="40"/>
+      <c r="C71" s="40"/>
+      <c r="D71" s="40"/>
+      <c r="E71" s="40"/>
+      <c r="F71" s="40"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="39" t="s">
+        <v>185</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="39" t="s">
+        <v>186</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+    </row>
+    <row r="75" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+    </row>
+    <row r="76" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+    </row>
+    <row r="77" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+    </row>
+    <row r="78" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+    </row>
+    <row r="79" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="39" t="s">
+        <v>191</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="39"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+    </row>
+    <row r="82" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+    </row>
+    <row r="83" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+    </row>
+    <row r="85" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+    </row>
+    <row r="86" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="50"/>
+      <c r="B86" s="13"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+    </row>
+    <row r="87" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="50"/>
+      <c r="B87" s="13"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+    </row>
+    <row r="88" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="50"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+    </row>
+    <row r="89" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="50"/>
+      <c r="B89" s="13"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
+    </row>
+    <row r="90" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="50"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
+    </row>
+    <row r="91" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="50"/>
+      <c r="B91" s="13"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="13"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="B93" s="54"/>
+      <c r="C93" s="54"/>
+      <c r="D93" s="54"/>
+      <c r="E93" s="54"/>
+      <c r="F93" s="54"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="B94" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C94" s="55" t="s">
+        <v>110</v>
+      </c>
+      <c r="D94" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="E94" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="F94" s="55" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="B95" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="C95" s="55"/>
+      <c r="D95" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="E95" s="55"/>
+      <c r="F95" s="55"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="C96" s="55"/>
+      <c r="D96" s="55"/>
+      <c r="E96" s="55"/>
+      <c r="F96" s="55"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="56" t="s">
+        <v>162</v>
+      </c>
+      <c r="B97" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C97" s="55"/>
+      <c r="D97" s="55"/>
+      <c r="E97" s="55"/>
+      <c r="F97" s="55"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="B103" s="49"/>
+      <c r="C103" s="49"/>
+      <c r="D103" s="49"/>
+      <c r="E103" s="49"/>
+      <c r="F103" s="49"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="B104" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C104" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D104" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E104" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="F104" s="37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="B74" s="48"/>
-      <c r="C74" s="48"/>
-      <c r="D74" s="48"/>
-      <c r="E74" s="48"/>
-      <c r="F74" s="48"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="45" t="s">
+      <c r="B105" s="38"/>
+      <c r="C105" s="38"/>
+      <c r="D105" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="E105" s="38"/>
+      <c r="F105" s="38"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" s="49" t="s">
+        <v>170</v>
+      </c>
+      <c r="B117" s="49"/>
+      <c r="C117" s="49"/>
+      <c r="D117" s="49"/>
+      <c r="E117" s="49"/>
+      <c r="F117" s="49"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="B75" s="45" t="s">
+      <c r="B118" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="C75" s="45" t="s">
+      <c r="C118" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="D75" s="45" t="s">
+      <c r="D118" s="37" t="s">
         <v>111</v>
       </c>
-      <c r="E75" s="45" t="s">
+      <c r="E118" s="37" t="s">
         <v>112</v>
       </c>
-      <c r="F75" s="45" t="s">
+      <c r="F118" s="37" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="46" t="s">
-        <v>153</v>
-      </c>
-      <c r="B76" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C76" s="46"/>
-      <c r="D76" s="46" t="s">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="B119" s="38"/>
+      <c r="C119" s="38"/>
+      <c r="D119" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="E76" s="46"/>
-      <c r="F76" s="46"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="48" t="s">
-        <v>166</v>
-      </c>
-      <c r="B84" s="48"/>
-      <c r="C84" s="48"/>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="B85" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="C85" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="D85" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E85" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F85" s="45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="46" t="s">
-        <v>167</v>
-      </c>
-      <c r="B86" s="46"/>
-      <c r="C86" s="46"/>
-      <c r="D86" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="E86" s="46"/>
-      <c r="F86" s="46"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B88" s="3"/>
-      <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
+      <c r="E119" s="38"/>
+      <c r="F119" s="38"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="48" t="s">
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+      <c r="D121" s="3"/>
+      <c r="E121" s="3"/>
+      <c r="F121" s="3"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B98" s="48"/>
-      <c r="C98" s="48"/>
-      <c r="D98" s="48"/>
-      <c r="E98" s="48"/>
-      <c r="F98" s="48"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="B99" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="C99" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="D99" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E99" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F99" s="45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="46" t="s">
+      <c r="B122" s="2"/>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B100" s="46"/>
-      <c r="C100" s="46"/>
-      <c r="D100" s="46" t="s">
-        <v>109</v>
-      </c>
-      <c r="E100" s="46"/>
-      <c r="F100" s="46"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
+      <c r="B124" s="2"/>
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A117:F117"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A30:F30"/>
     <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A53:F53"/>
-    <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A74:F74"/>
-    <mergeCell ref="A84:F84"/>
+    <mergeCell ref="A54:F54"/>
+    <mergeCell ref="A66:F66"/>
+    <mergeCell ref="A93:F93"/>
+    <mergeCell ref="A103:F103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>